<commit_message>
Fixed mislabel in form
</commit_message>
<xml_diff>
--- a/extras/test-form/Text, integer, decimal test form.xlsx
+++ b/extras/test-form/Text, integer, decimal test form.xlsx
@@ -5,12 +5,12 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/max.s.haberman/Documents/SurveyCTO code/Field plug-ins by Max/In progress/text-integer-decimal/extras/sample-form/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/max.s.haberman/Documents/SurveyCTO code/Field plug-ins by Max/In progress/text-integer-decimal/extras/test-form/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80B415F7-6D1A-5347-9A07-CA1924055CBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53C6C0F4-B822-BD4C-8BBB-05D77206CDDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28080" yWindow="1380" windowWidth="25000" windowHeight="15540" tabRatio="534" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28440" yWindow="500" windowWidth="25000" windowHeight="15540" tabRatio="534" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="555" uniqueCount="379">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="575" uniqueCount="391">
   <si>
     <t>deviceid</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -188,9 +188,6 @@
     <t>note</t>
   </si>
   <si>
-    <t>intronote</t>
-  </si>
-  <si>
     <t>response_note</t>
   </si>
   <si>
@@ -2411,76 +2408,6 @@
     <t>username</t>
   </si>
   <si>
-    <t>q1</t>
-  </si>
-  <si>
-    <t>This is an example question, which asks the user to enter some text.</t>
-  </si>
-  <si>
-    <t>q2</t>
-  </si>
-  <si>
-    <t>This is another example question, which asks the user to enter a number.</t>
-  </si>
-  <si>
-    <t>select_one yesno</t>
-  </si>
-  <si>
-    <t>q3</t>
-  </si>
-  <si>
-    <t>This is another example question, which asks the user to select yes or no. The options and their labels are on the choices worksheet.</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">This is a note field, which displays something to the user. 
-The fields above this one are hidden ones, auto-filled by SurveyCTO; they collect information that is often useful to have in your data. The fields below are just a few examples. Please feel free to delete them.
-You can customize this form (perhaps something simple to start, like changing some of these labels), then you can upload it to your SurveyCTO server console by clicking </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Upload form </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">on the </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Design </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>tab.</t>
-    </r>
-  </si>
-  <si>
     <t>value</t>
   </si>
   <si>
@@ -2677,13 +2604,76 @@
   </si>
   <si>
     <t>text_integer_decimal_test_form</t>
+  </si>
+  <si>
+    <t>default_text</t>
+  </si>
+  <si>
+    <t>text_numbers</t>
+  </si>
+  <si>
+    <t>text_numbers_decimal</t>
+  </si>
+  <si>
+    <t>This is a standard &lt;em&gt;text&lt;/em&gt; field.</t>
+  </si>
+  <si>
+    <t>This &lt;em&gt;text&lt;/em&gt; field has the "numbers_phone" &lt;em&gt;appearance&lt;/em&gt;.</t>
+  </si>
+  <si>
+    <t>text_numbers_phone</t>
+  </si>
+  <si>
+    <t>This &lt;em&gt;text&lt;/em&gt; field has the "numbers" &lt;em&gt;appearance&lt;/em&gt;.</t>
+  </si>
+  <si>
+    <t>This &lt;em&gt;text&lt;/em&gt; field has the "numbers_decimal" &lt;em&gt;appearance&lt;/em&gt;.</t>
+  </si>
+  <si>
+    <t>default_integer</t>
+  </si>
+  <si>
+    <t>This is a standard &lt;em&gt;integer&lt;/em&gt; field.</t>
+  </si>
+  <si>
+    <t>This &lt;em&gt;integer&lt;/em&gt; field has the "show_formatted" &lt;em&gt;appearance&lt;/em&gt;.</t>
+  </si>
+  <si>
+    <t>This &lt;em&gt;decimal&lt;/em&gt; field has the "show_formatted" &lt;em&gt;appearance&lt;/em&gt;.</t>
+  </si>
+  <si>
+    <t>integer_formatted</t>
+  </si>
+  <si>
+    <t>default_decimal</t>
+  </si>
+  <si>
+    <t>decimal_formatted</t>
+  </si>
+  <si>
+    <t>numbers_phone custom-text-integer-decimal</t>
+  </si>
+  <si>
+    <t>custom-text-integer-decimal</t>
+  </si>
+  <si>
+    <t>numbers custom-text-integer-decimal</t>
+  </si>
+  <si>
+    <t>numbers_decimal custom-text-integer-decimal</t>
+  </si>
+  <si>
+    <t>show_formatted custom-text-integer-decimal</t>
+  </si>
+  <si>
+    <t>This is a standard &lt;em&gt;decimal&lt;/em&gt; field.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color indexed="8"/>
@@ -2802,14 +2792,6 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="12"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="8">
@@ -4834,13 +4816,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W15"/>
+  <dimension ref="A1:W19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A12" sqref="A12"/>
+      <selection pane="bottomRight" activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4926,19 +4908,19 @@
         <v>14</v>
       </c>
       <c r="S1" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="T1" s="5" t="s">
         <v>42</v>
       </c>
       <c r="U1" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="V1" s="5" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="W1" s="5" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.2">
@@ -5001,33 +4983,33 @@
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="I8" s="11"/>
       <c r="J8" s="11"/>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A9" s="9" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="I9" s="11"/>
       <c r="J9" s="11"/>
       <c r="N9" s="9" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A10" s="9" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="I10" s="11"/>
       <c r="J10" s="11"/>
@@ -5036,50 +5018,118 @@
       <c r="I11" s="11"/>
       <c r="J11" s="11"/>
     </row>
-    <row r="12" spans="1:23" ht="306" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:23" ht="34" x14ac:dyDescent="0.2">
       <c r="A12" s="9" t="s">
-        <v>42</v>
+        <v>96</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>43</v>
+        <v>370</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>314</v>
+        <v>373</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>386</v>
       </c>
       <c r="I12" s="11"/>
       <c r="J12" s="11"/>
     </row>
-    <row r="13" spans="1:23" ht="34" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:23" ht="51" x14ac:dyDescent="0.2">
       <c r="A13" s="9" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>307</v>
+        <v>375</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>308</v>
+        <v>374</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>385</v>
       </c>
     </row>
     <row r="14" spans="1:23" ht="51" x14ac:dyDescent="0.2">
       <c r="A14" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>371</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>376</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" ht="51" x14ac:dyDescent="0.2">
+      <c r="A15" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>372</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>377</v>
+      </c>
+      <c r="F15" s="9" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" ht="34" x14ac:dyDescent="0.2">
+      <c r="A16" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>378</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>379</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="A17" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>382</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>380</v>
+      </c>
+      <c r="F17" s="9" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="A18" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="B14" s="9" t="s">
-        <v>309</v>
-      </c>
-      <c r="C14" s="10" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="15" spans="1:23" ht="68" x14ac:dyDescent="0.2">
-      <c r="A15" s="9" t="s">
-        <v>311</v>
-      </c>
-      <c r="B15" s="9" t="s">
-        <v>312</v>
-      </c>
-      <c r="C15" s="10" t="s">
-        <v>313</v>
+      <c r="B18" s="9" t="s">
+        <v>383</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>390</v>
+      </c>
+      <c r="F18" s="9" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="A19" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>384</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>381</v>
+      </c>
+      <c r="F19" s="9" t="s">
+        <v>389</v>
       </c>
     </row>
   </sheetData>
@@ -5249,7 +5299,7 @@
         <v>26</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
       <c r="C1" s="13" t="s">
         <v>25</v>
@@ -5258,7 +5308,7 @@
         <v>27</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -5374,20 +5424,20 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="17" t="s">
-        <v>377</v>
+        <v>368</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>378</v>
+        <v>369</v>
       </c>
       <c r="C2" s="17" t="str">
         <f ca="1">TEXT(YEAR(NOW())-2000, "00") &amp; TEXT(MONTH(NOW()), "00") &amp; TEXT(DAY(NOW()), "00") &amp; TEXT(HOUR(NOW()), "00") &amp; TEXT(MINUTE(NOW()), "00")</f>
-        <v>2108052004</v>
+        <v>2108052125</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>376</v>
+        <v>367</v>
       </c>
       <c r="E2" s="19" t="s">
-        <v>376</v>
+        <v>367</v>
       </c>
       <c r="F2" s="17" t="s">
         <v>29</v>
@@ -5417,7 +5467,7 @@
   <sheetData>
     <row r="1" spans="1:30" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="53" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B1" s="54"/>
       <c r="C1" s="32"/>
@@ -5429,7 +5479,7 @@
     </row>
     <row r="3" spans="1:30" s="33" customFormat="1" ht="97" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="57" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B3" s="58"/>
       <c r="C3" s="32"/>
@@ -5448,13 +5498,13 @@
         <v>25</v>
       </c>
       <c r="D5" s="35" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E5" s="34" t="s">
         <v>7</v>
       </c>
       <c r="F5" s="34" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G5" s="34" t="s">
         <v>5</v>
@@ -5463,19 +5513,19 @@
         <v>8</v>
       </c>
       <c r="I5" s="34" t="s">
-        <v>318</v>
+        <v>309</v>
       </c>
       <c r="J5" s="35" t="s">
         <v>41</v>
       </c>
       <c r="K5" s="35" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="L5" s="34" t="s">
-        <v>319</v>
+        <v>310</v>
       </c>
       <c r="M5" s="34" t="s">
-        <v>320</v>
+        <v>311</v>
       </c>
       <c r="N5" s="34" t="s">
         <v>11</v>
@@ -5484,141 +5534,141 @@
         <v>40</v>
       </c>
       <c r="P5" s="34" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="Q5" s="34" t="s">
         <v>12</v>
       </c>
       <c r="R5" s="34" t="s">
-        <v>321</v>
+        <v>312</v>
       </c>
       <c r="S5" s="34" t="s">
         <v>39</v>
       </c>
       <c r="T5" s="34" t="s">
-        <v>322</v>
+        <v>313</v>
       </c>
       <c r="U5" s="34" t="s">
         <v>13</v>
       </c>
       <c r="V5" s="34" t="s">
-        <v>323</v>
+        <v>314</v>
       </c>
       <c r="W5" s="34" t="s">
+        <v>70</v>
+      </c>
+      <c r="X5" s="34" t="s">
         <v>71</v>
       </c>
-      <c r="X5" s="34" t="s">
+      <c r="Y5" s="34" t="s">
         <v>72</v>
       </c>
-      <c r="Y5" s="34" t="s">
-        <v>73</v>
-      </c>
       <c r="Z5" s="34" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="AA5" s="34" t="s">
         <v>42</v>
       </c>
       <c r="AB5" s="34" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AC5" s="34" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="AD5" s="34" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="6" spans="1:30" s="39" customFormat="1" ht="221" x14ac:dyDescent="0.2">
       <c r="A6" s="38" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B6" s="38" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C6" s="38" t="s">
+        <v>73</v>
+      </c>
+      <c r="D6" s="38" t="s">
+        <v>62</v>
+      </c>
+      <c r="E6" s="38" t="s">
         <v>74</v>
       </c>
-      <c r="D6" s="38" t="s">
-        <v>63</v>
-      </c>
-      <c r="E6" s="38" t="s">
+      <c r="F6" s="38" t="s">
+        <v>88</v>
+      </c>
+      <c r="G6" s="38" t="s">
         <v>75</v>
       </c>
-      <c r="F6" s="38" t="s">
+      <c r="H6" s="38" t="s">
+        <v>76</v>
+      </c>
+      <c r="I6" s="38" t="s">
+        <v>274</v>
+      </c>
+      <c r="J6" s="38" t="s">
+        <v>77</v>
+      </c>
+      <c r="K6" s="38" t="s">
         <v>89</v>
       </c>
-      <c r="G6" s="38" t="s">
-        <v>76</v>
-      </c>
-      <c r="H6" s="38" t="s">
-        <v>77</v>
-      </c>
-      <c r="I6" s="38" t="s">
+      <c r="L6" s="38" t="s">
+        <v>273</v>
+      </c>
+      <c r="M6" s="38" t="s">
+        <v>78</v>
+      </c>
+      <c r="N6" s="38" t="s">
+        <v>79</v>
+      </c>
+      <c r="O6" s="38" t="s">
+        <v>80</v>
+      </c>
+      <c r="P6" s="38" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q6" s="38" t="s">
+        <v>81</v>
+      </c>
+      <c r="R6" s="38" t="s">
         <v>275</v>
       </c>
-      <c r="J6" s="38" t="s">
-        <v>78</v>
-      </c>
-      <c r="K6" s="38" t="s">
-        <v>90</v>
-      </c>
-      <c r="L6" s="38" t="s">
-        <v>274</v>
-      </c>
-      <c r="M6" s="38" t="s">
-        <v>79</v>
-      </c>
-      <c r="N6" s="38" t="s">
-        <v>80</v>
-      </c>
-      <c r="O6" s="38" t="s">
-        <v>81</v>
-      </c>
-      <c r="P6" s="38" t="s">
+      <c r="S6" s="38" t="s">
+        <v>82</v>
+      </c>
+      <c r="T6" s="38" t="s">
+        <v>84</v>
+      </c>
+      <c r="U6" s="38" t="s">
+        <v>85</v>
+      </c>
+      <c r="V6" s="38" t="s">
+        <v>86</v>
+      </c>
+      <c r="W6" s="38" t="s">
         <v>91</v>
       </c>
-      <c r="Q6" s="38" t="s">
-        <v>82</v>
-      </c>
-      <c r="R6" s="38" t="s">
-        <v>276</v>
-      </c>
-      <c r="S6" s="38" t="s">
-        <v>83</v>
-      </c>
-      <c r="T6" s="38" t="s">
-        <v>85</v>
-      </c>
-      <c r="U6" s="38" t="s">
-        <v>86</v>
-      </c>
-      <c r="V6" s="38" t="s">
+      <c r="X6" s="38" t="s">
+        <v>92</v>
+      </c>
+      <c r="Y6" s="38" t="s">
+        <v>93</v>
+      </c>
+      <c r="Z6" s="38" t="s">
         <v>87</v>
       </c>
-      <c r="W6" s="38" t="s">
-        <v>92</v>
-      </c>
-      <c r="X6" s="38" t="s">
-        <v>93</v>
-      </c>
-      <c r="Y6" s="38" t="s">
+      <c r="AA6" s="38" t="s">
         <v>94</v>
       </c>
-      <c r="Z6" s="38" t="s">
-        <v>88</v>
-      </c>
-      <c r="AA6" s="38" t="s">
+      <c r="AB6" s="38" t="s">
         <v>95</v>
       </c>
-      <c r="AB6" s="38" t="s">
-        <v>96</v>
-      </c>
       <c r="AC6" s="38" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="AD6" s="38" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="7" spans="1:30" s="33" customFormat="1" x14ac:dyDescent="0.2">
@@ -5626,7 +5676,7 @@
     </row>
     <row r="8" spans="1:30" s="42" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="59" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B8" s="59"/>
       <c r="C8" s="40"/>
@@ -5663,13 +5713,13 @@
     </row>
     <row r="10" spans="1:30" s="45" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="43" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B10" s="43" t="s">
+        <v>98</v>
+      </c>
+      <c r="C10" s="44" t="s">
         <v>99</v>
-      </c>
-      <c r="C10" s="44" t="s">
-        <v>100</v>
       </c>
       <c r="D10" s="43"/>
       <c r="E10" s="43"/>
@@ -5701,20 +5751,20 @@
     </row>
     <row r="11" spans="1:30" s="45" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="43" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B11" s="43" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C11" s="44" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D11" s="43"/>
       <c r="E11" s="43"/>
       <c r="F11" s="43"/>
       <c r="G11" s="43"/>
       <c r="H11" s="43" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I11" s="43"/>
       <c r="J11" s="43"/>
@@ -5741,13 +5791,13 @@
     </row>
     <row r="12" spans="1:30" s="45" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="43" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B12" s="43" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C12" s="44" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D12" s="43"/>
       <c r="E12" s="43"/>
@@ -5779,13 +5829,13 @@
     </row>
     <row r="13" spans="1:30" s="45" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="43" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B13" s="43" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C13" s="44" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D13" s="43"/>
       <c r="E13" s="43"/>
@@ -5817,13 +5867,13 @@
     </row>
     <row r="14" spans="1:30" s="45" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A14" s="43" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B14" s="43" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C14" s="44" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D14" s="43"/>
       <c r="E14" s="43"/>
@@ -5855,20 +5905,20 @@
     </row>
     <row r="15" spans="1:30" s="45" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A15" s="43" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B15" s="43" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C15" s="44" t="s">
-        <v>369</v>
+        <v>360</v>
       </c>
       <c r="D15" s="43"/>
       <c r="E15" s="43"/>
       <c r="F15" s="43"/>
       <c r="G15" s="43"/>
       <c r="H15" s="43" t="s">
-        <v>366</v>
+        <v>357</v>
       </c>
       <c r="I15" s="43"/>
       <c r="J15" s="43"/>
@@ -5895,20 +5945,20 @@
     </row>
     <row r="16" spans="1:30" s="45" customFormat="1" ht="68" x14ac:dyDescent="0.2">
       <c r="A16" s="43" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B16" s="43" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C16" s="44" t="s">
-        <v>370</v>
+        <v>361</v>
       </c>
       <c r="D16" s="43"/>
       <c r="E16" s="43"/>
       <c r="F16" s="43"/>
       <c r="G16" s="43"/>
       <c r="H16" s="43" t="s">
-        <v>367</v>
+        <v>358</v>
       </c>
       <c r="I16" s="43"/>
       <c r="J16" s="43"/>
@@ -5935,20 +5985,20 @@
     </row>
     <row r="17" spans="1:30" s="45" customFormat="1" ht="68" x14ac:dyDescent="0.2">
       <c r="A17" s="43" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B17" s="43" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C17" s="44" t="s">
-        <v>371</v>
+        <v>362</v>
       </c>
       <c r="D17" s="43"/>
       <c r="E17" s="43"/>
       <c r="F17" s="43"/>
       <c r="G17" s="43"/>
       <c r="H17" s="43" t="s">
-        <v>368</v>
+        <v>359</v>
       </c>
       <c r="I17" s="43"/>
       <c r="J17" s="43"/>
@@ -5975,20 +6025,20 @@
     </row>
     <row r="18" spans="1:30" s="45" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A18" s="43" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B18" s="43" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C18" s="44" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D18" s="43"/>
       <c r="E18" s="43"/>
       <c r="F18" s="43"/>
       <c r="G18" s="43"/>
       <c r="H18" s="43" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I18" s="43"/>
       <c r="J18" s="43"/>
@@ -6015,20 +6065,20 @@
     </row>
     <row r="19" spans="1:30" s="45" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A19" s="43" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B19" s="43" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C19" s="44" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D19" s="43"/>
       <c r="E19" s="43"/>
       <c r="F19" s="43"/>
       <c r="G19" s="43"/>
       <c r="H19" s="43" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I19" s="43"/>
       <c r="J19" s="43"/>
@@ -6055,20 +6105,20 @@
     </row>
     <row r="20" spans="1:30" s="45" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A20" s="43" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B20" s="43" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C20" s="44" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D20" s="43"/>
       <c r="E20" s="43"/>
       <c r="F20" s="43"/>
       <c r="G20" s="43"/>
       <c r="H20" s="43" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I20" s="43"/>
       <c r="J20" s="43"/>
@@ -6095,20 +6145,20 @@
     </row>
     <row r="21" spans="1:30" s="45" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A21" s="43" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B21" s="43" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C21" s="44" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D21" s="43"/>
       <c r="E21" s="43"/>
       <c r="F21" s="43"/>
       <c r="G21" s="43"/>
       <c r="H21" s="43" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I21" s="43"/>
       <c r="J21" s="43"/>
@@ -6135,20 +6185,20 @@
     </row>
     <row r="22" spans="1:30" s="45" customFormat="1" ht="68" x14ac:dyDescent="0.2">
       <c r="A22" s="43" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B22" s="43" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C22" s="44" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D22" s="43"/>
       <c r="E22" s="43"/>
       <c r="F22" s="43"/>
       <c r="G22" s="43"/>
       <c r="H22" s="43" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I22" s="43"/>
       <c r="J22" s="43"/>
@@ -6175,20 +6225,20 @@
     </row>
     <row r="23" spans="1:30" s="45" customFormat="1" ht="85" x14ac:dyDescent="0.2">
       <c r="A23" s="43" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B23" s="43" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C23" s="44" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D23" s="43"/>
       <c r="E23" s="43"/>
       <c r="F23" s="43"/>
       <c r="G23" s="43"/>
       <c r="H23" s="43" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I23" s="43"/>
       <c r="J23" s="43"/>
@@ -6215,20 +6265,20 @@
     </row>
     <row r="24" spans="1:30" s="45" customFormat="1" ht="68" x14ac:dyDescent="0.2">
       <c r="A24" s="43" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B24" s="43" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C24" s="44" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D24" s="43"/>
       <c r="E24" s="43"/>
       <c r="F24" s="43"/>
       <c r="G24" s="43"/>
       <c r="H24" s="43" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="I24" s="43"/>
       <c r="J24" s="43"/>
@@ -6255,20 +6305,20 @@
     </row>
     <row r="25" spans="1:30" s="45" customFormat="1" ht="68" x14ac:dyDescent="0.2">
       <c r="A25" s="43" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B25" s="43" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C25" s="44" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D25" s="43"/>
       <c r="E25" s="43"/>
       <c r="F25" s="43"/>
       <c r="G25" s="43"/>
       <c r="H25" s="43" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="I25" s="43"/>
       <c r="J25" s="43"/>
@@ -6295,20 +6345,20 @@
     </row>
     <row r="26" spans="1:30" s="45" customFormat="1" ht="68" x14ac:dyDescent="0.2">
       <c r="A26" s="43" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B26" s="43" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C26" s="52" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D26" s="43"/>
       <c r="E26" s="43"/>
       <c r="F26" s="43"/>
       <c r="G26" s="43"/>
       <c r="H26" s="43" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="I26" s="43"/>
       <c r="J26" s="43"/>
@@ -6335,20 +6385,20 @@
     </row>
     <row r="27" spans="1:30" s="45" customFormat="1" ht="68" x14ac:dyDescent="0.2">
       <c r="A27" s="43" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B27" s="43" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C27" s="44" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D27" s="43"/>
       <c r="E27" s="43"/>
       <c r="F27" s="43"/>
       <c r="G27" s="43"/>
       <c r="H27" s="43" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="I27" s="43"/>
       <c r="J27" s="43"/>
@@ -6375,20 +6425,20 @@
     </row>
     <row r="28" spans="1:30" s="45" customFormat="1" ht="85" x14ac:dyDescent="0.2">
       <c r="A28" s="43" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B28" s="43" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C28" s="44" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D28" s="43"/>
       <c r="E28" s="43"/>
       <c r="F28" s="43"/>
       <c r="G28" s="43"/>
       <c r="H28" s="43" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="I28" s="43"/>
       <c r="J28" s="43"/>
@@ -6415,13 +6465,13 @@
     </row>
     <row r="29" spans="1:30" s="45" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A29" s="43" t="s">
+        <v>112</v>
+      </c>
+      <c r="B29" s="43" t="s">
+        <v>98</v>
+      </c>
+      <c r="C29" s="44" t="s">
         <v>113</v>
-      </c>
-      <c r="B29" s="43" t="s">
-        <v>99</v>
-      </c>
-      <c r="C29" s="44" t="s">
-        <v>114</v>
       </c>
       <c r="D29" s="43"/>
       <c r="E29" s="43"/>
@@ -6453,20 +6503,20 @@
     </row>
     <row r="30" spans="1:30" s="45" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A30" s="43" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B30" s="43" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C30" s="44" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D30" s="43"/>
       <c r="E30" s="43"/>
       <c r="F30" s="43"/>
       <c r="G30" s="43"/>
       <c r="H30" s="43" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I30" s="43"/>
       <c r="J30" s="43"/>
@@ -6493,20 +6543,20 @@
     </row>
     <row r="31" spans="1:30" s="45" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A31" s="43" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B31" s="43" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C31" s="44" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D31" s="43"/>
       <c r="E31" s="43"/>
       <c r="F31" s="43"/>
       <c r="G31" s="43"/>
       <c r="H31" s="43" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I31" s="43"/>
       <c r="J31" s="43"/>
@@ -6533,20 +6583,20 @@
     </row>
     <row r="32" spans="1:30" s="45" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A32" s="43" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B32" s="43" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C32" s="44" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D32" s="43"/>
       <c r="E32" s="43"/>
       <c r="F32" s="43"/>
       <c r="G32" s="43"/>
       <c r="H32" s="43" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I32" s="43"/>
       <c r="J32" s="43"/>
@@ -6573,20 +6623,20 @@
     </row>
     <row r="33" spans="1:30" s="45" customFormat="1" ht="68" x14ac:dyDescent="0.2">
       <c r="A33" s="43" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B33" s="43" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C33" s="44" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D33" s="43"/>
       <c r="E33" s="43"/>
       <c r="F33" s="43"/>
       <c r="G33" s="43"/>
       <c r="H33" s="43" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="I33" s="43"/>
       <c r="J33" s="43"/>
@@ -6613,20 +6663,20 @@
     </row>
     <row r="34" spans="1:30" s="45" customFormat="1" ht="68" x14ac:dyDescent="0.2">
       <c r="A34" s="43" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B34" s="43" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C34" s="44" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D34" s="43"/>
       <c r="E34" s="43"/>
       <c r="F34" s="43"/>
       <c r="G34" s="43"/>
       <c r="H34" s="43" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="I34" s="43"/>
       <c r="J34" s="43"/>
@@ -6653,20 +6703,20 @@
     </row>
     <row r="35" spans="1:30" s="45" customFormat="1" ht="68" x14ac:dyDescent="0.2">
       <c r="A35" s="43" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B35" s="43" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C35" s="52" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="D35" s="43"/>
       <c r="E35" s="43"/>
       <c r="F35" s="43"/>
       <c r="G35" s="43"/>
       <c r="H35" s="43" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="I35" s="43"/>
       <c r="J35" s="43"/>
@@ -6693,20 +6743,20 @@
     </row>
     <row r="36" spans="1:30" s="45" customFormat="1" ht="68" x14ac:dyDescent="0.2">
       <c r="A36" s="43" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B36" s="43" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C36" s="44" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D36" s="43"/>
       <c r="E36" s="43"/>
       <c r="F36" s="43"/>
       <c r="G36" s="43"/>
       <c r="H36" s="43" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="I36" s="43"/>
       <c r="J36" s="43"/>
@@ -6733,20 +6783,20 @@
     </row>
     <row r="37" spans="1:30" s="45" customFormat="1" ht="85" x14ac:dyDescent="0.2">
       <c r="A37" s="43" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B37" s="43" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C37" s="44" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D37" s="43"/>
       <c r="E37" s="43"/>
       <c r="F37" s="43"/>
       <c r="G37" s="43"/>
       <c r="H37" s="43" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="I37" s="43"/>
       <c r="J37" s="43"/>
@@ -6773,13 +6823,13 @@
     </row>
     <row r="38" spans="1:30" s="45" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A38" s="43" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B38" s="43" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C38" s="44" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D38" s="43"/>
       <c r="E38" s="43"/>
@@ -6811,13 +6861,13 @@
     </row>
     <row r="39" spans="1:30" s="45" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A39" s="43" t="s">
-        <v>324</v>
+        <v>315</v>
       </c>
       <c r="B39" s="43" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C39" s="44" t="s">
-        <v>325</v>
+        <v>316</v>
       </c>
       <c r="D39" s="43"/>
       <c r="E39" s="43"/>
@@ -6849,13 +6899,13 @@
     </row>
     <row r="40" spans="1:30" s="45" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A40" s="43" t="s">
-        <v>326</v>
+        <v>317</v>
       </c>
       <c r="B40" s="43" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C40" s="44" t="s">
-        <v>327</v>
+        <v>318</v>
       </c>
       <c r="D40" s="43"/>
       <c r="E40" s="43"/>
@@ -6887,13 +6937,13 @@
     </row>
     <row r="41" spans="1:30" s="45" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A41" s="43" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B41" s="43" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C41" s="44" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D41" s="43"/>
       <c r="E41" s="43"/>
@@ -6925,13 +6975,13 @@
     </row>
     <row r="42" spans="1:30" s="45" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A42" s="43" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B42" s="43" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C42" s="44" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D42" s="43"/>
       <c r="E42" s="43"/>
@@ -6963,20 +7013,20 @@
     </row>
     <row r="43" spans="1:30" s="45" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A43" s="43" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B43" s="43" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C43" s="44" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D43" s="43"/>
       <c r="E43" s="43"/>
       <c r="F43" s="43"/>
       <c r="G43" s="43"/>
       <c r="H43" s="43" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I43" s="43"/>
       <c r="J43" s="43"/>
@@ -7003,13 +7053,13 @@
     </row>
     <row r="44" spans="1:30" s="45" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A44" s="43" t="s">
+        <v>132</v>
+      </c>
+      <c r="B44" s="43" t="s">
+        <v>98</v>
+      </c>
+      <c r="C44" s="44" t="s">
         <v>133</v>
-      </c>
-      <c r="B44" s="43" t="s">
-        <v>99</v>
-      </c>
-      <c r="C44" s="44" t="s">
-        <v>134</v>
       </c>
       <c r="D44" s="43"/>
       <c r="E44" s="43"/>
@@ -7041,20 +7091,20 @@
     </row>
     <row r="45" spans="1:30" s="45" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A45" s="43" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B45" s="43" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C45" s="44" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D45" s="43"/>
       <c r="E45" s="43"/>
       <c r="F45" s="43"/>
       <c r="G45" s="43"/>
       <c r="H45" s="43" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I45" s="43"/>
       <c r="J45" s="43"/>
@@ -7084,10 +7134,10 @@
         <v>27</v>
       </c>
       <c r="B46" s="43" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C46" s="44" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D46" s="43"/>
       <c r="E46" s="43"/>
@@ -7122,17 +7172,17 @@
         <v>27</v>
       </c>
       <c r="B47" s="43" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C47" s="44" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D47" s="43"/>
       <c r="E47" s="43"/>
       <c r="F47" s="43"/>
       <c r="G47" s="43"/>
       <c r="H47" s="43" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="I47" s="43"/>
       <c r="J47" s="43"/>
@@ -7162,17 +7212,17 @@
         <v>27</v>
       </c>
       <c r="B48" s="43" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C48" s="44" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D48" s="43"/>
       <c r="E48" s="43"/>
       <c r="F48" s="43"/>
       <c r="G48" s="43"/>
       <c r="H48" s="43" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="I48" s="43"/>
       <c r="J48" s="43"/>
@@ -7202,17 +7252,17 @@
         <v>27</v>
       </c>
       <c r="B49" s="43" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C49" s="44" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D49" s="43"/>
       <c r="E49" s="43"/>
       <c r="F49" s="43"/>
       <c r="G49" s="43"/>
       <c r="H49" s="43" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="I49" s="43"/>
       <c r="J49" s="43"/>
@@ -7239,13 +7289,13 @@
     </row>
     <row r="50" spans="1:30" s="45" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A50" s="43" t="s">
+        <v>142</v>
+      </c>
+      <c r="B50" s="43" t="s">
+        <v>98</v>
+      </c>
+      <c r="C50" s="44" t="s">
         <v>143</v>
-      </c>
-      <c r="B50" s="43" t="s">
-        <v>99</v>
-      </c>
-      <c r="C50" s="44" t="s">
-        <v>144</v>
       </c>
       <c r="D50" s="43"/>
       <c r="E50" s="43"/>
@@ -7277,13 +7327,13 @@
     </row>
     <row r="51" spans="1:30" s="45" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A51" s="43" t="s">
+        <v>144</v>
+      </c>
+      <c r="B51" s="43" t="s">
+        <v>98</v>
+      </c>
+      <c r="C51" s="44" t="s">
         <v>145</v>
-      </c>
-      <c r="B51" s="43" t="s">
-        <v>99</v>
-      </c>
-      <c r="C51" s="44" t="s">
-        <v>146</v>
       </c>
       <c r="D51" s="43"/>
       <c r="E51" s="43"/>
@@ -7315,13 +7365,13 @@
     </row>
     <row r="52" spans="1:30" s="45" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A52" s="43" t="s">
-        <v>316</v>
+        <v>307</v>
       </c>
       <c r="B52" s="43" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C52" s="44" t="s">
-        <v>317</v>
+        <v>308</v>
       </c>
       <c r="D52" s="43"/>
       <c r="E52" s="43"/>
@@ -7356,10 +7406,10 @@
         <v>42</v>
       </c>
       <c r="B53" s="43" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C53" s="44" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D53" s="43"/>
       <c r="E53" s="43"/>
@@ -7394,7 +7444,7 @@
         <v>33</v>
       </c>
       <c r="B54" s="43" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C54" s="44"/>
       <c r="D54" s="43"/>
@@ -7430,7 +7480,7 @@
         <v>34</v>
       </c>
       <c r="B55" s="43" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C55" s="44"/>
       <c r="D55" s="43"/>
@@ -7466,7 +7516,7 @@
         <v>35</v>
       </c>
       <c r="B56" s="43" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C56" s="44"/>
       <c r="D56" s="43"/>
@@ -7502,7 +7552,7 @@
         <v>36</v>
       </c>
       <c r="B57" s="43" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C57" s="44"/>
       <c r="D57" s="43"/>
@@ -7538,7 +7588,7 @@
         <v>38</v>
       </c>
       <c r="B58" s="43" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C58" s="44"/>
       <c r="D58" s="43"/>
@@ -7571,10 +7621,10 @@
     </row>
     <row r="59" spans="1:30" s="45" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A59" s="43" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B59" s="43" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C59" s="44"/>
       <c r="D59" s="43"/>
@@ -7610,7 +7660,7 @@
         <v>37</v>
       </c>
       <c r="B60" s="43" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C60" s="44"/>
       <c r="D60" s="43"/>
@@ -7643,10 +7693,10 @@
     </row>
     <row r="61" spans="1:30" s="45" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A61" s="43" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B61" s="43" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C61" s="44"/>
       <c r="D61" s="43"/>
@@ -7679,10 +7729,10 @@
     </row>
     <row r="62" spans="1:30" s="45" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A62" s="43" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B62" s="43" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C62" s="44"/>
       <c r="D62" s="43"/>
@@ -7700,7 +7750,7 @@
       <c r="P62" s="43"/>
       <c r="Q62" s="43"/>
       <c r="R62" s="43" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="S62" s="43"/>
       <c r="T62" s="43"/>
@@ -7717,10 +7767,10 @@
     </row>
     <row r="63" spans="1:30" s="45" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A63" s="43" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B63" s="43" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C63" s="44"/>
       <c r="D63" s="43"/>
@@ -7738,7 +7788,7 @@
       <c r="P63" s="43"/>
       <c r="Q63" s="43"/>
       <c r="R63" s="43" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="S63" s="43"/>
       <c r="T63" s="43"/>
@@ -7755,10 +7805,10 @@
     </row>
     <row r="64" spans="1:30" s="45" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A64" s="43" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B64" s="43" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C64" s="44"/>
       <c r="D64" s="43"/>
@@ -7766,7 +7816,7 @@
       <c r="F64" s="43"/>
       <c r="G64" s="43"/>
       <c r="H64" s="43" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="I64" s="43"/>
       <c r="J64" s="43"/>
@@ -7793,10 +7843,10 @@
     </row>
     <row r="65" spans="1:30" s="45" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A65" s="43" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B65" s="43" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C65" s="44"/>
       <c r="D65" s="43"/>
@@ -7804,7 +7854,7 @@
       <c r="F65" s="43"/>
       <c r="G65" s="43"/>
       <c r="H65" s="43" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I65" s="43"/>
       <c r="J65" s="43"/>
@@ -7831,10 +7881,10 @@
     </row>
     <row r="66" spans="1:30" s="45" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A66" s="43" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B66" s="43" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C66" s="44"/>
       <c r="D66" s="43"/>
@@ -7842,7 +7892,7 @@
       <c r="F66" s="43"/>
       <c r="G66" s="43"/>
       <c r="H66" s="43" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="I66" s="43"/>
       <c r="J66" s="43"/>
@@ -7869,10 +7919,10 @@
     </row>
     <row r="67" spans="1:30" s="45" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A67" s="43" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B67" s="43" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C67" s="44"/>
       <c r="D67" s="43"/>
@@ -7880,7 +7930,7 @@
       <c r="F67" s="43"/>
       <c r="G67" s="43"/>
       <c r="H67" s="43" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I67" s="43"/>
       <c r="J67" s="43"/>
@@ -7907,13 +7957,13 @@
     </row>
     <row r="68" spans="1:30" s="45" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A68" s="43" t="s">
+        <v>158</v>
+      </c>
+      <c r="B68" s="43" t="s">
+        <v>161</v>
+      </c>
+      <c r="C68" s="44" t="s">
         <v>159</v>
-      </c>
-      <c r="B68" s="43" t="s">
-        <v>162</v>
-      </c>
-      <c r="C68" s="44" t="s">
-        <v>160</v>
       </c>
       <c r="D68" s="43"/>
       <c r="E68" s="43"/>
@@ -7945,7 +7995,7 @@
     </row>
     <row r="69" spans="1:30" s="45" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A69" s="43" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B69" s="43"/>
       <c r="C69" s="44"/>
@@ -7979,10 +8029,10 @@
     </row>
     <row r="70" spans="1:30" s="45" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A70" s="43" t="s">
+        <v>160</v>
+      </c>
+      <c r="B70" s="43" t="s">
         <v>161</v>
-      </c>
-      <c r="B70" s="43" t="s">
-        <v>162</v>
       </c>
       <c r="C70" s="44"/>
       <c r="D70" s="43"/>
@@ -8015,13 +8065,13 @@
     </row>
     <row r="71" spans="1:30" s="45" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A71" s="43" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B71" s="43" t="s">
+        <v>165</v>
+      </c>
+      <c r="C71" s="44" t="s">
         <v>166</v>
-      </c>
-      <c r="C71" s="44" t="s">
-        <v>167</v>
       </c>
       <c r="D71" s="43"/>
       <c r="E71" s="43"/>
@@ -8053,7 +8103,7 @@
     </row>
     <row r="72" spans="1:30" s="45" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A72" s="43" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B72" s="43"/>
       <c r="C72" s="44"/>
@@ -8087,10 +8137,10 @@
     </row>
     <row r="73" spans="1:30" s="45" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A73" s="43" t="s">
+        <v>164</v>
+      </c>
+      <c r="B73" s="43" t="s">
         <v>165</v>
-      </c>
-      <c r="B73" s="43" t="s">
-        <v>166</v>
       </c>
       <c r="C73" s="44"/>
       <c r="D73" s="43"/>
@@ -8123,13 +8173,13 @@
     </row>
     <row r="74" spans="1:30" s="45" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A74" s="43" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B74" s="43" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C74" s="44" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D74" s="43"/>
       <c r="E74" s="43"/>
@@ -8163,7 +8213,7 @@
     </row>
     <row r="75" spans="1:30" s="45" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A75" s="43" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B75" s="43"/>
       <c r="C75" s="44"/>
@@ -8197,10 +8247,10 @@
     </row>
     <row r="76" spans="1:30" s="45" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A76" s="43" t="s">
+        <v>164</v>
+      </c>
+      <c r="B76" s="43" t="s">
         <v>165</v>
-      </c>
-      <c r="B76" s="43" t="s">
-        <v>166</v>
       </c>
       <c r="C76" s="44"/>
       <c r="D76" s="43"/>
@@ -8233,10 +8283,10 @@
     </row>
     <row r="77" spans="1:30" s="45" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A77" s="43" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B77" s="43" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C77" s="44"/>
       <c r="D77" s="43"/>
@@ -8269,10 +8319,10 @@
     </row>
     <row r="78" spans="1:30" s="45" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A78" s="43" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B78" s="43" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C78" s="44"/>
       <c r="D78" s="43"/>
@@ -8305,10 +8355,10 @@
     </row>
     <row r="79" spans="1:30" s="45" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A79" s="43" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B79" s="43" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C79" s="44"/>
       <c r="D79" s="43"/>
@@ -8316,7 +8366,7 @@
       <c r="F79" s="43"/>
       <c r="G79" s="43"/>
       <c r="H79" s="43" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="I79" s="43"/>
       <c r="J79" s="43"/>
@@ -8343,10 +8393,10 @@
     </row>
     <row r="80" spans="1:30" s="45" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A80" s="43" t="s">
-        <v>372</v>
+        <v>363</v>
       </c>
       <c r="B80" s="43" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C80" s="44"/>
       <c r="D80" s="43"/>
@@ -8354,7 +8404,7 @@
       <c r="F80" s="43"/>
       <c r="G80" s="43"/>
       <c r="H80" s="43" t="s">
-        <v>373</v>
+        <v>364</v>
       </c>
       <c r="I80" s="43"/>
       <c r="J80" s="43"/>
@@ -8381,10 +8431,10 @@
     </row>
     <row r="81" spans="1:30" s="45" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A81" s="43" t="s">
-        <v>374</v>
+        <v>365</v>
       </c>
       <c r="B81" s="43" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C81" s="44"/>
       <c r="D81" s="43"/>
@@ -8392,7 +8442,7 @@
       <c r="F81" s="43"/>
       <c r="G81" s="43"/>
       <c r="H81" s="43" t="s">
-        <v>375</v>
+        <v>366</v>
       </c>
       <c r="I81" s="43"/>
       <c r="J81" s="43"/>
@@ -8419,7 +8469,7 @@
     </row>
     <row r="83" spans="1:30" s="31" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A83" s="60" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B83" s="61"/>
       <c r="C83" s="26"/>
@@ -8453,27 +8503,27 @@
     </row>
     <row r="85" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A85" s="22" t="s">
+        <v>168</v>
+      </c>
+      <c r="B85" s="22" t="s">
         <v>169</v>
       </c>
-      <c r="B85" s="22" t="s">
+      <c r="C85" s="22" t="s">
         <v>170</v>
       </c>
-      <c r="C85" s="22" t="s">
+      <c r="D85" s="22" t="s">
         <v>171</v>
-      </c>
-      <c r="D85" s="22" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="86" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A86" s="23" t="s">
+        <v>172</v>
+      </c>
+      <c r="B86" s="23" t="s">
         <v>173</v>
       </c>
-      <c r="B86" s="23" t="s">
+      <c r="C86" s="23" t="s">
         <v>174</v>
-      </c>
-      <c r="C86" s="23" t="s">
-        <v>175</v>
       </c>
       <c r="D86" s="23">
         <v>2</v>
@@ -8481,10 +8531,10 @@
     </row>
     <row r="87" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A87" s="23" t="s">
+        <v>175</v>
+      </c>
+      <c r="B87" s="23" t="s">
         <v>176</v>
-      </c>
-      <c r="B87" s="23" t="s">
-        <v>177</v>
       </c>
       <c r="C87" s="24" t="str">
         <f>"3 - 2"</f>
@@ -8496,13 +8546,13 @@
     </row>
     <row r="88" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A88" s="23" t="s">
+        <v>177</v>
+      </c>
+      <c r="B88" s="23" t="s">
         <v>178</v>
       </c>
-      <c r="B88" s="23" t="s">
+      <c r="C88" s="23" t="s">
         <v>179</v>
-      </c>
-      <c r="C88" s="23" t="s">
-        <v>180</v>
       </c>
       <c r="D88" s="23">
         <v>6</v>
@@ -8510,13 +8560,13 @@
     </row>
     <row r="89" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A89" s="23" t="s">
+        <v>180</v>
+      </c>
+      <c r="B89" s="23" t="s">
         <v>181</v>
       </c>
-      <c r="B89" s="23" t="s">
+      <c r="C89" s="23" t="s">
         <v>182</v>
-      </c>
-      <c r="C89" s="23" t="s">
-        <v>183</v>
       </c>
       <c r="D89" s="23">
         <v>5</v>
@@ -8524,13 +8574,13 @@
     </row>
     <row r="90" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A90" s="23" t="s">
+        <v>183</v>
+      </c>
+      <c r="B90" s="23" t="s">
         <v>184</v>
       </c>
-      <c r="B90" s="23" t="s">
+      <c r="C90" s="23" t="s">
         <v>185</v>
-      </c>
-      <c r="C90" s="23" t="s">
-        <v>186</v>
       </c>
       <c r="D90" s="23">
         <v>1</v>
@@ -8538,128 +8588,128 @@
     </row>
     <row r="91" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A91" s="23" t="s">
+        <v>186</v>
+      </c>
+      <c r="B91" s="23" t="s">
         <v>187</v>
       </c>
-      <c r="B91" s="23" t="s">
+      <c r="C91" s="23" t="s">
         <v>188</v>
       </c>
-      <c r="C91" s="23" t="s">
+      <c r="D91" s="23" t="s">
         <v>189</v>
-      </c>
-      <c r="D91" s="23" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="92" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A92" s="23" t="s">
+        <v>190</v>
+      </c>
+      <c r="B92" s="23" t="s">
         <v>191</v>
       </c>
-      <c r="B92" s="23" t="s">
+      <c r="C92" s="23" t="s">
         <v>192</v>
       </c>
-      <c r="C92" s="23" t="s">
-        <v>193</v>
-      </c>
       <c r="D92" s="23" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="93" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A93" s="23" t="s">
+        <v>193</v>
+      </c>
+      <c r="B93" s="23" t="s">
         <v>194</v>
       </c>
-      <c r="B93" s="23" t="s">
+      <c r="C93" s="23" t="s">
         <v>195</v>
       </c>
-      <c r="C93" s="23" t="s">
-        <v>196</v>
-      </c>
       <c r="D93" s="23" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="94" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A94" s="23" t="s">
+        <v>196</v>
+      </c>
+      <c r="B94" s="23" t="s">
         <v>197</v>
       </c>
-      <c r="B94" s="23" t="s">
+      <c r="C94" s="23" t="s">
         <v>198</v>
       </c>
-      <c r="C94" s="23" t="s">
-        <v>199</v>
-      </c>
       <c r="D94" s="23" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="95" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A95" s="23" t="s">
+        <v>199</v>
+      </c>
+      <c r="B95" s="23" t="s">
         <v>200</v>
       </c>
-      <c r="B95" s="23" t="s">
+      <c r="C95" s="23" t="s">
         <v>201</v>
       </c>
-      <c r="C95" s="23" t="s">
-        <v>202</v>
-      </c>
       <c r="D95" s="23" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="96" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A96" s="23" t="s">
+        <v>202</v>
+      </c>
+      <c r="B96" s="23" t="s">
         <v>203</v>
       </c>
-      <c r="B96" s="23" t="s">
+      <c r="C96" s="23" t="s">
         <v>204</v>
       </c>
-      <c r="C96" s="23" t="s">
-        <v>205</v>
-      </c>
       <c r="D96" s="23" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A97" s="23" t="s">
+        <v>205</v>
+      </c>
+      <c r="B97" s="23" t="s">
         <v>206</v>
       </c>
-      <c r="B97" s="23" t="s">
+      <c r="C97" s="23" t="s">
         <v>207</v>
       </c>
-      <c r="C97" s="23" t="s">
-        <v>208</v>
-      </c>
       <c r="D97" s="23" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A98" s="23" t="s">
+        <v>208</v>
+      </c>
+      <c r="B98" s="23" t="s">
         <v>209</v>
       </c>
-      <c r="B98" s="23" t="s">
+      <c r="C98" s="23" t="s">
         <v>210</v>
       </c>
-      <c r="C98" s="23" t="s">
-        <v>211</v>
-      </c>
       <c r="D98" s="23" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A99" s="23" t="s">
+        <v>211</v>
+      </c>
+      <c r="B99" s="23" t="s">
         <v>212</v>
       </c>
-      <c r="B99" s="23" t="s">
+      <c r="C99" s="23" t="s">
         <v>213</v>
       </c>
-      <c r="C99" s="23" t="s">
+      <c r="D99" s="23" t="s">
         <v>214</v>
-      </c>
-      <c r="D99" s="23" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.2">
@@ -8671,540 +8721,540 @@
     <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A101" s="25"/>
       <c r="B101" s="22" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C101" s="22" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D101" s="25"/>
     </row>
     <row r="102" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A102" s="25"/>
       <c r="B102" s="27" t="s">
+        <v>216</v>
+      </c>
+      <c r="C102" s="28" t="s">
         <v>217</v>
-      </c>
-      <c r="C102" s="28" t="s">
-        <v>218</v>
       </c>
       <c r="D102" s="25"/>
     </row>
     <row r="103" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A103" s="25"/>
       <c r="B103" s="28" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C103" s="28" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D103" s="25"/>
     </row>
     <row r="104" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A104" s="25"/>
       <c r="B104" s="28" t="s">
+        <v>218</v>
+      </c>
+      <c r="C104" s="28" t="s">
         <v>219</v>
-      </c>
-      <c r="C104" s="28" t="s">
-        <v>220</v>
       </c>
       <c r="D104" s="25"/>
     </row>
     <row r="105" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A105" s="25"/>
       <c r="B105" s="28" t="s">
+        <v>220</v>
+      </c>
+      <c r="C105" s="28" t="s">
         <v>221</v>
-      </c>
-      <c r="C105" s="28" t="s">
-        <v>222</v>
       </c>
       <c r="D105" s="25"/>
     </row>
     <row r="106" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A106" s="25"/>
       <c r="B106" s="28" t="s">
+        <v>222</v>
+      </c>
+      <c r="C106" s="28" t="s">
         <v>223</v>
-      </c>
-      <c r="C106" s="28" t="s">
-        <v>224</v>
       </c>
       <c r="D106" s="25"/>
     </row>
     <row r="107" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A107" s="25"/>
       <c r="B107" s="28" t="s">
+        <v>224</v>
+      </c>
+      <c r="C107" s="28" t="s">
         <v>225</v>
-      </c>
-      <c r="C107" s="28" t="s">
-        <v>226</v>
       </c>
       <c r="D107" s="25"/>
     </row>
     <row r="108" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A108" s="25"/>
       <c r="B108" s="28" t="s">
+        <v>226</v>
+      </c>
+      <c r="C108" s="28" t="s">
         <v>227</v>
-      </c>
-      <c r="C108" s="28" t="s">
-        <v>228</v>
       </c>
       <c r="D108" s="25"/>
     </row>
     <row r="109" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A109" s="25"/>
       <c r="B109" s="28" t="s">
+        <v>228</v>
+      </c>
+      <c r="C109" s="28" t="s">
         <v>229</v>
-      </c>
-      <c r="C109" s="28" t="s">
-        <v>230</v>
       </c>
       <c r="D109" s="25"/>
     </row>
     <row r="110" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A110" s="25"/>
       <c r="B110" s="28" t="s">
+        <v>230</v>
+      </c>
+      <c r="C110" s="28" t="s">
         <v>231</v>
-      </c>
-      <c r="C110" s="28" t="s">
-        <v>232</v>
       </c>
       <c r="D110" s="25"/>
     </row>
     <row r="111" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A111" s="25"/>
       <c r="B111" s="28" t="s">
-        <v>328</v>
+        <v>319</v>
       </c>
       <c r="C111" s="28" t="s">
-        <v>328</v>
+        <v>319</v>
       </c>
       <c r="D111" s="25"/>
     </row>
     <row r="112" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A112" s="25"/>
       <c r="B112" s="28" t="s">
+        <v>232</v>
+      </c>
+      <c r="C112" s="28" t="s">
         <v>233</v>
-      </c>
-      <c r="C112" s="28" t="s">
-        <v>234</v>
       </c>
       <c r="D112" s="25"/>
     </row>
     <row r="113" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A113" s="25"/>
       <c r="B113" s="28" t="s">
+        <v>234</v>
+      </c>
+      <c r="C113" s="28" t="s">
         <v>235</v>
-      </c>
-      <c r="C113" s="28" t="s">
-        <v>236</v>
       </c>
       <c r="D113" s="25"/>
     </row>
     <row r="114" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A114" s="25"/>
       <c r="B114" s="28" t="s">
+        <v>236</v>
+      </c>
+      <c r="C114" s="28" t="s">
         <v>237</v>
-      </c>
-      <c r="C114" s="28" t="s">
-        <v>238</v>
       </c>
       <c r="D114" s="25"/>
     </row>
     <row r="115" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A115" s="25"/>
       <c r="B115" s="28" t="s">
+        <v>238</v>
+      </c>
+      <c r="C115" s="28" t="s">
         <v>239</v>
-      </c>
-      <c r="C115" s="28" t="s">
-        <v>240</v>
       </c>
       <c r="D115" s="25"/>
     </row>
     <row r="116" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A116" s="25"/>
       <c r="B116" s="28" t="s">
+        <v>240</v>
+      </c>
+      <c r="C116" s="28" t="s">
         <v>241</v>
-      </c>
-      <c r="C116" s="28" t="s">
-        <v>242</v>
       </c>
       <c r="D116" s="25"/>
     </row>
     <row r="117" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A117" s="25"/>
       <c r="B117" s="28" t="s">
+        <v>242</v>
+      </c>
+      <c r="C117" s="28" t="s">
         <v>243</v>
-      </c>
-      <c r="C117" s="28" t="s">
-        <v>244</v>
       </c>
       <c r="D117" s="25"/>
     </row>
     <row r="118" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A118" s="25"/>
       <c r="B118" s="28" t="s">
+        <v>244</v>
+      </c>
+      <c r="C118" s="28" t="s">
         <v>245</v>
-      </c>
-      <c r="C118" s="28" t="s">
-        <v>246</v>
       </c>
       <c r="D118" s="25"/>
     </row>
     <row r="119" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A119" s="25"/>
       <c r="B119" s="28" t="s">
+        <v>246</v>
+      </c>
+      <c r="C119" s="28" t="s">
         <v>247</v>
-      </c>
-      <c r="C119" s="28" t="s">
-        <v>248</v>
       </c>
       <c r="D119" s="25"/>
     </row>
     <row r="120" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A120" s="25"/>
       <c r="B120" s="28" t="s">
+        <v>248</v>
+      </c>
+      <c r="C120" s="28" t="s">
         <v>249</v>
-      </c>
-      <c r="C120" s="28" t="s">
-        <v>250</v>
       </c>
       <c r="D120" s="25"/>
     </row>
     <row r="121" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A121" s="25"/>
       <c r="B121" s="28" t="s">
+        <v>250</v>
+      </c>
+      <c r="C121" s="28" t="s">
         <v>251</v>
-      </c>
-      <c r="C121" s="28" t="s">
-        <v>252</v>
       </c>
       <c r="D121" s="25"/>
     </row>
     <row r="122" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A122" s="25"/>
       <c r="B122" s="28" t="s">
+        <v>252</v>
+      </c>
+      <c r="C122" s="28" t="s">
         <v>253</v>
-      </c>
-      <c r="C122" s="28" t="s">
-        <v>254</v>
       </c>
       <c r="D122" s="25"/>
     </row>
     <row r="123" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A123" s="25"/>
       <c r="B123" s="28" t="s">
+        <v>254</v>
+      </c>
+      <c r="C123" s="28" t="s">
         <v>255</v>
-      </c>
-      <c r="C123" s="28" t="s">
-        <v>256</v>
       </c>
       <c r="D123" s="25"/>
     </row>
     <row r="124" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A124" s="25"/>
       <c r="B124" s="28" t="s">
+        <v>256</v>
+      </c>
+      <c r="C124" s="28" t="s">
         <v>257</v>
-      </c>
-      <c r="C124" s="28" t="s">
-        <v>258</v>
       </c>
       <c r="D124" s="25"/>
     </row>
     <row r="125" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A125" s="25"/>
       <c r="B125" s="28" t="s">
+        <v>258</v>
+      </c>
+      <c r="C125" s="28" t="s">
         <v>259</v>
-      </c>
-      <c r="C125" s="28" t="s">
-        <v>260</v>
       </c>
       <c r="D125" s="25"/>
     </row>
     <row r="126" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A126" s="25"/>
       <c r="B126" s="28" t="s">
+        <v>260</v>
+      </c>
+      <c r="C126" s="28" t="s">
         <v>261</v>
-      </c>
-      <c r="C126" s="28" t="s">
-        <v>262</v>
       </c>
       <c r="D126" s="25"/>
     </row>
     <row r="127" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A127" s="25"/>
       <c r="B127" s="28" t="s">
+        <v>262</v>
+      </c>
+      <c r="C127" s="28" t="s">
         <v>263</v>
-      </c>
-      <c r="C127" s="28" t="s">
-        <v>264</v>
       </c>
       <c r="D127" s="25"/>
     </row>
     <row r="128" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A128" s="25"/>
       <c r="B128" s="28" t="s">
+        <v>264</v>
+      </c>
+      <c r="C128" s="28" t="s">
         <v>265</v>
-      </c>
-      <c r="C128" s="28" t="s">
-        <v>266</v>
       </c>
       <c r="D128" s="25"/>
     </row>
     <row r="129" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A129" s="25"/>
       <c r="B129" s="29" t="s">
+        <v>266</v>
+      </c>
+      <c r="C129" s="29" t="s">
         <v>267</v>
-      </c>
-      <c r="C129" s="29" t="s">
-        <v>268</v>
       </c>
       <c r="D129" s="25"/>
     </row>
     <row r="130" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A130" s="25"/>
       <c r="B130" s="29" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C130" s="29" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D130" s="25"/>
     </row>
     <row r="131" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A131" s="25"/>
       <c r="B131" s="29" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C131" s="29" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D131" s="25"/>
     </row>
     <row r="132" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A132" s="25"/>
       <c r="B132" s="29" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C132" s="29" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D132" s="25"/>
     </row>
     <row r="133" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A133" s="25"/>
       <c r="B133" s="29" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C133" s="29" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D133" s="25"/>
     </row>
     <row r="134" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A134" s="25"/>
       <c r="B134" s="29" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C134" s="29" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D134" s="25"/>
     </row>
     <row r="135" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A135" s="25"/>
       <c r="B135" s="29" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C135" s="29" t="s">
-        <v>329</v>
+        <v>320</v>
       </c>
       <c r="D135" s="25"/>
     </row>
     <row r="136" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A136" s="25"/>
       <c r="B136" s="29" t="s">
-        <v>330</v>
+        <v>321</v>
       </c>
       <c r="C136" s="29" t="s">
-        <v>330</v>
+        <v>321</v>
       </c>
       <c r="D136" s="25"/>
     </row>
     <row r="137" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A137" s="25"/>
       <c r="B137" s="29" t="s">
-        <v>331</v>
+        <v>322</v>
       </c>
       <c r="C137" s="29" t="s">
-        <v>332</v>
+        <v>323</v>
       </c>
       <c r="D137" s="25"/>
     </row>
     <row r="138" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A138" s="25"/>
       <c r="B138" s="29" t="s">
-        <v>333</v>
+        <v>324</v>
       </c>
       <c r="C138" s="29" t="s">
-        <v>334</v>
+        <v>325</v>
       </c>
       <c r="D138" s="25"/>
     </row>
     <row r="139" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A139" s="25"/>
       <c r="B139" s="29" t="s">
-        <v>335</v>
+        <v>326</v>
       </c>
       <c r="C139" s="29" t="s">
-        <v>336</v>
+        <v>327</v>
       </c>
       <c r="D139" s="25"/>
     </row>
     <row r="140" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A140" s="25"/>
       <c r="B140" s="29" t="s">
-        <v>337</v>
+        <v>328</v>
       </c>
       <c r="C140" s="29" t="s">
-        <v>338</v>
+        <v>329</v>
       </c>
       <c r="D140" s="25"/>
     </row>
     <row r="141" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A141" s="25"/>
       <c r="B141" s="29" t="s">
-        <v>339</v>
+        <v>330</v>
       </c>
       <c r="C141" s="29" t="s">
-        <v>340</v>
+        <v>331</v>
       </c>
       <c r="D141" s="25"/>
     </row>
     <row r="142" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A142" s="25"/>
       <c r="B142" s="29" t="s">
-        <v>341</v>
+        <v>332</v>
       </c>
       <c r="C142" s="29" t="s">
-        <v>342</v>
+        <v>333</v>
       </c>
       <c r="D142" s="25"/>
     </row>
     <row r="143" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A143" s="25"/>
       <c r="B143" s="29" t="s">
-        <v>343</v>
+        <v>334</v>
       </c>
       <c r="C143" s="29" t="s">
-        <v>344</v>
+        <v>335</v>
       </c>
       <c r="D143" s="25"/>
     </row>
     <row r="144" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A144" s="25"/>
       <c r="B144" s="29" t="s">
-        <v>345</v>
+        <v>336</v>
       </c>
       <c r="C144" s="29" t="s">
-        <v>346</v>
+        <v>337</v>
       </c>
       <c r="D144" s="25"/>
     </row>
     <row r="145" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A145" s="25"/>
       <c r="B145" s="29" t="s">
-        <v>347</v>
+        <v>338</v>
       </c>
       <c r="C145" s="29" t="s">
-        <v>348</v>
+        <v>339</v>
       </c>
       <c r="D145" s="25"/>
     </row>
     <row r="146" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A146" s="25"/>
       <c r="B146" s="29" t="s">
-        <v>349</v>
+        <v>340</v>
       </c>
       <c r="C146" s="29" t="s">
-        <v>350</v>
+        <v>341</v>
       </c>
       <c r="D146" s="25"/>
     </row>
     <row r="147" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A147" s="25"/>
       <c r="B147" s="29" t="s">
-        <v>351</v>
+        <v>342</v>
       </c>
       <c r="C147" s="29" t="s">
-        <v>352</v>
+        <v>343</v>
       </c>
       <c r="D147" s="25"/>
     </row>
     <row r="148" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A148" s="25"/>
       <c r="B148" s="29" t="s">
-        <v>353</v>
+        <v>344</v>
       </c>
       <c r="C148" s="29" t="s">
-        <v>354</v>
+        <v>345</v>
       </c>
       <c r="D148" s="25"/>
     </row>
     <row r="149" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A149" s="25"/>
       <c r="B149" s="29" t="s">
-        <v>355</v>
+        <v>346</v>
       </c>
       <c r="C149" s="29" t="s">
-        <v>356</v>
+        <v>347</v>
       </c>
       <c r="D149" s="25"/>
     </row>
     <row r="150" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A150" s="25"/>
       <c r="B150" s="29" t="s">
-        <v>357</v>
+        <v>348</v>
       </c>
       <c r="C150" s="29" t="s">
-        <v>358</v>
+        <v>349</v>
       </c>
       <c r="D150" s="25"/>
     </row>
     <row r="151" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A151" s="25"/>
       <c r="B151" s="29" t="s">
-        <v>359</v>
+        <v>350</v>
       </c>
       <c r="C151" s="29" t="s">
-        <v>360</v>
+        <v>351</v>
       </c>
       <c r="D151" s="25"/>
     </row>
     <row r="152" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A152" s="25"/>
       <c r="B152" s="29" t="s">
-        <v>361</v>
+        <v>352</v>
       </c>
       <c r="C152" s="29" t="s">
-        <v>362</v>
+        <v>353</v>
       </c>
       <c r="D152" s="25"/>
     </row>
     <row r="153" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A153" s="25"/>
       <c r="B153" s="29" t="s">
-        <v>363</v>
+        <v>354</v>
       </c>
       <c r="C153" s="29" t="s">
-        <v>364</v>
+        <v>355</v>
       </c>
       <c r="D153" s="25"/>
     </row>
     <row r="154" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A154" s="25"/>
       <c r="B154" s="29" t="s">
-        <v>365</v>
+        <v>356</v>
       </c>
       <c r="C154" s="29" t="s">
-        <v>365</v>
+        <v>356</v>
       </c>
       <c r="D154" s="25"/>
     </row>
@@ -9582,7 +9632,7 @@
   <sheetData>
     <row r="1" spans="1:8" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="53" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B1" s="54"/>
     </row>
@@ -9592,7 +9642,7 @@
     </row>
     <row r="3" spans="1:8" s="33" customFormat="1" ht="99" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="57" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B3" s="58"/>
     </row>
@@ -9602,45 +9652,45 @@
         <v>26</v>
       </c>
       <c r="B5" s="47" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
       <c r="C5" s="48" t="s">
         <v>25</v>
       </c>
       <c r="D5" s="48" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E5" s="47" t="s">
         <v>27</v>
       </c>
       <c r="F5" s="47" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G5" s="47" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:8" s="39" customFormat="1" ht="221" x14ac:dyDescent="0.2">
       <c r="A6" s="38" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B6" s="38" t="s">
+        <v>58</v>
+      </c>
+      <c r="C6" s="38" t="s">
         <v>59</v>
       </c>
-      <c r="C6" s="38" t="s">
-        <v>60</v>
-      </c>
       <c r="D6" s="38" t="s">
+        <v>62</v>
+      </c>
+      <c r="E6" s="38" t="s">
+        <v>83</v>
+      </c>
+      <c r="F6" s="38" t="s">
         <v>63</v>
       </c>
-      <c r="E6" s="38" t="s">
-        <v>84</v>
-      </c>
-      <c r="F6" s="38" t="s">
+      <c r="G6" s="38" t="s">
         <v>64</v>
-      </c>
-      <c r="G6" s="38" t="s">
-        <v>65</v>
       </c>
       <c r="H6" s="38"/>
     </row>
@@ -9670,7 +9720,7 @@
   <sheetData>
     <row r="1" spans="1:8" s="33" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="62" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B1" s="63"/>
       <c r="C1" s="49"/>
@@ -9688,7 +9738,7 @@
     </row>
     <row r="3" spans="1:8" s="33" customFormat="1" ht="55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="57" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B3" s="58"/>
       <c r="C3" s="49"/>
@@ -9727,22 +9777,22 @@
     </row>
     <row r="6" spans="1:8" s="39" customFormat="1" ht="340" x14ac:dyDescent="0.2">
       <c r="A6" s="38" t="s">
+        <v>48</v>
+      </c>
+      <c r="B6" s="38" t="s">
         <v>49</v>
       </c>
-      <c r="B6" s="38" t="s">
+      <c r="C6" s="38" t="s">
         <v>50</v>
       </c>
-      <c r="C6" s="38" t="s">
+      <c r="D6" s="38" t="s">
         <v>51</v>
       </c>
-      <c r="D6" s="38" t="s">
+      <c r="E6" s="38" t="s">
         <v>52</v>
       </c>
-      <c r="E6" s="38" t="s">
+      <c r="F6" s="38" t="s">
         <v>53</v>
-      </c>
-      <c r="F6" s="38" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Added inputmode parameters to form
</commit_message>
<xml_diff>
--- a/extras/test-form/Text, integer, decimal test form.xlsx
+++ b/extras/test-form/Text, integer, decimal test form.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/max.s.haberman/Documents/SurveyCTO code/Field plug-ins by Max/In progress/text-integer-decimal/extras/test-form/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53C6C0F4-B822-BD4C-8BBB-05D77206CDDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E12CE7E6-9B48-7445-990F-02DA2174F926}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28440" yWindow="500" windowWidth="25000" windowHeight="15540" tabRatio="534" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28360" yWindow="500" windowWidth="25000" windowHeight="15540" tabRatio="534" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="575" uniqueCount="391">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="579" uniqueCount="394">
   <si>
     <t>deviceid</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -2667,6 +2667,17 @@
   </si>
   <si>
     <t>This is a standard &lt;em&gt;decimal&lt;/em&gt; field.</t>
+  </si>
+  <si>
+    <t>custom-text-integer-decimal(inputmode-ios='numeric', inputmode-android='numeric', inputmode-web='numeric')</t>
+  </si>
+  <si>
+    <t>inputmode</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;This &lt;em&gt;text&lt;/em&gt; field has this &lt;em&gt;appearance&lt;/em&gt;:&lt;/p&gt;
+&lt;p&gt;&lt;code&gt;custom-text-integer-decimal(inputmode-ios='numeric', inputmode-android='numeric', inputmode-web='numeric')&lt;/code&gt;&lt;/p&gt;
+&lt;p&gt;That way, it will always show a numeric keyboard, even though it is a text field.&lt;/p&gt;</t>
   </si>
 </sst>
 </file>
@@ -4816,13 +4827,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W19"/>
+  <dimension ref="A1:W21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A20" sqref="A20"/>
+      <selection pane="bottomRight" activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5132,6 +5143,20 @@
         <v>389</v>
       </c>
     </row>
+    <row r="21" spans="1:6" ht="170" x14ac:dyDescent="0.2">
+      <c r="A21" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>392</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>393</v>
+      </c>
+      <c r="F21" s="9" t="s">
+        <v>391</v>
+      </c>
+    </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -5431,7 +5456,7 @@
       </c>
       <c r="C2" s="17" t="str">
         <f ca="1">TEXT(YEAR(NOW())-2000, "00") &amp; TEXT(MONTH(NOW()), "00") &amp; TEXT(DAY(NOW()), "00") &amp; TEXT(HOUR(NOW()), "00") &amp; TEXT(MINUTE(NOW()), "00")</f>
-        <v>2108052125</v>
+        <v>2108092352</v>
       </c>
       <c r="D2" s="18" t="s">
         <v>367</v>
@@ -6023,7 +6048,7 @@
       <c r="AC17" s="43"/>
       <c r="AD17" s="43"/>
     </row>
-    <row r="18" spans="1:30" s="45" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:30" s="45" customFormat="1" ht="68" x14ac:dyDescent="0.2">
       <c r="A18" s="43" t="s">
         <v>102</v>
       </c>

</xml_diff>